<commit_message>
adding folded by dimension matrix.added viz fixing. P values printing
</commit_message>
<xml_diff>
--- a/data/Grapes-Vineyard B.xlsx
+++ b/data/Grapes-Vineyard B.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matan.lindenbaum/PycharmProjects/pythonProject/pythonProject2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95E6BC0-5555-DF4E-B7D7-B5F6A494C033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C84DA0-DDCE-7F4F-B710-2FED1D4641ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38380" yWindow="500" windowWidth="38380" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$631</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -545,7 +548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH631"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
       <selection activeCell="AB8" sqref="AB8"/>
     </sheetView>
   </sheetViews>
@@ -63928,14 +63931,18 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:P631" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -64110,27 +64117,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C305EC0A-6C7C-4514-9751-D865437D03A0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD870983-5326-4F33-918E-4B0FF063D598}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="76caa081-fc44-4d2c-bd81-6f9a75f04feb"/>
-    <ds:schemaRef ds:uri="0a540cde-0ccb-4e9b-9eab-821ccdced025"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -64155,9 +64150,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD870983-5326-4F33-918E-4B0FF063D598}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C305EC0A-6C7C-4514-9751-D865437D03A0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="76caa081-fc44-4d2c-bd81-6f9a75f04feb"/>
+    <ds:schemaRef ds:uri="0a540cde-0ccb-4e9b-9eab-821ccdced025"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>